<commit_message>
written stockitem script oct18
</commit_message>
<xml_diff>
--- a/FileInput/Controller.xlsx
+++ b/FileInput/Controller.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8304" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8304" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestCases" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Suppliers" sheetId="4" r:id="rId4"/>
     <sheet name="Cusstomers" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="86">
   <si>
     <t>TCID</t>
   </si>
@@ -167,6 +167,120 @@
   </si>
   <si>
     <t>closeBrowser</t>
+  </si>
+  <si>
+    <t>Wait for stock item link</t>
+  </si>
+  <si>
+    <t>Click Stock items link</t>
+  </si>
+  <si>
+    <t>//a[text()='Stock Items ']</t>
+  </si>
+  <si>
+    <t>Wait for Add Icon</t>
+  </si>
+  <si>
+    <t>Click Add icon</t>
+  </si>
+  <si>
+    <t>(//span[@data-caption='Add'])[1]</t>
+  </si>
+  <si>
+    <t>Wait for Category Listbox</t>
+  </si>
+  <si>
+    <t>Select item in Category</t>
+  </si>
+  <si>
+    <t>dropDownAction</t>
+  </si>
+  <si>
+    <t>Seelct item in Supplier Number</t>
+  </si>
+  <si>
+    <t>x_Category</t>
+  </si>
+  <si>
+    <t>//select[@id='x_Category']</t>
+  </si>
+  <si>
+    <t>x_Supplier_Number</t>
+  </si>
+  <si>
+    <t>Capture Stock number</t>
+  </si>
+  <si>
+    <t>captureStock</t>
+  </si>
+  <si>
+    <t>x_Stock_Number</t>
+  </si>
+  <si>
+    <t>Enter Stcok name</t>
+  </si>
+  <si>
+    <t>Puzzels</t>
+  </si>
+  <si>
+    <t>x_Stock_Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select item in Unit Of Measurement </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter Purchasing Price </t>
+  </si>
+  <si>
+    <t>Enter Selling Price</t>
+  </si>
+  <si>
+    <t>Enter notes</t>
+  </si>
+  <si>
+    <t>Selling Puzzles</t>
+  </si>
+  <si>
+    <t>x_Purchasing_Price</t>
+  </si>
+  <si>
+    <t>x_Unit_Of_Measurement</t>
+  </si>
+  <si>
+    <t>x_Selling_Price</t>
+  </si>
+  <si>
+    <t>x_Notes</t>
+  </si>
+  <si>
+    <t>Click add button</t>
+  </si>
+  <si>
+    <t>btnAction</t>
+  </si>
+  <si>
+    <t>Verify Stock Number</t>
+  </si>
+  <si>
+    <t>stockTable</t>
+  </si>
+  <si>
+    <t>Wait for Confirm ok button</t>
+  </si>
+  <si>
+    <t>Click Confirm ok button</t>
+  </si>
+  <si>
+    <t>//button[normalize-space()='OK!']</t>
+  </si>
+  <si>
+    <t>Wait for alert ok</t>
+  </si>
+  <si>
+    <t>Click Alert ok</t>
+  </si>
+  <si>
+    <t>(//button[starts-with(text(),'OK')])[6]</t>
   </si>
 </sst>
 </file>
@@ -255,12 +369,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,7 +649,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -544,7 +660,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -576,7 +692,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -588,7 +704,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -626,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -846,19 +962,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -881,6 +998,528 @@
       <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.6">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.6">
+      <c r="A3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.6">
+      <c r="A4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="4">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.6">
+      <c r="A5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.6">
+      <c r="A6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.6">
+      <c r="A7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.6">
+      <c r="A8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="4">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.6">
+      <c r="A9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.6">
+      <c r="A10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="6">
+        <v>10</v>
+      </c>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.6">
+      <c r="A11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.6">
+      <c r="A12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="6">
+        <v>10</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.6">
+      <c r="A13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.6">
+      <c r="A14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="6">
+        <v>10</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.6">
+      <c r="A15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.6">
+      <c r="A16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.6">
+      <c r="A17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.6">
+      <c r="A18" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.6">
+      <c r="A19" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.6">
+      <c r="A20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="5">
+        <v>300000</v>
+      </c>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.6">
+      <c r="A21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="5">
+        <v>500000</v>
+      </c>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.6">
+      <c r="A22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.6">
+      <c r="A23" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.6">
+      <c r="A24" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="5">
+        <v>10</v>
+      </c>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.6">
+      <c r="A25" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.6">
+      <c r="A26" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" s="5">
+        <v>10</v>
+      </c>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.6">
+      <c r="A27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.6">
+      <c r="A28" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.6">
+      <c r="A29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.6">
+      <c r="A30" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>